<commit_message>
Laatste verbetering van een regel
</commit_message>
<xml_diff>
--- a/Validatiematrix.xlsx
+++ b/Validatiematrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w.quak\Git\Geonovum\dso-validatiematrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC7B9FC-B22D-4E97-9814-AC074A19AADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43BBDEF-6A54-4E34-832C-15CF66AC04DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-12525" yWindow="-21720" windowWidth="51840" windowHeight="21120" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7863,13 +7863,13 @@
     <t>Het is niet mogelijk om een directe mutatie te doen op een ontwerpregeling.</t>
   </si>
   <si>
-    <t>Een te verwijderen wID in een RegelingMutatie MOET voorkomen in de was-versie.</t>
-  </si>
-  <si>
     <t>De volgende elementen binnen RegelingMetadata MOGEN NIET worden gewijzigd: Eindverantwoordelijke, Opvolging, SoortRegeling, Maker.</t>
   </si>
   <si>
     <t>De volgende elementen binnen InformatieobjectMetadata MOGEN NIET worden gewijzigd: Eindverantwoordelijke, FormaatInformatieobject, Opvolging, Publicatieinstructie, Maker.</t>
+  </si>
+  <si>
+    <t>De RegelingMutatie MAG GEEN te verwijderen wId's bevatten die niet voorkomen in de was-versie</t>
   </si>
 </sst>
 </file>
@@ -9408,11 +9408,11 @@
   <dimension ref="A1:K853"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C180" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C233" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="A3" sqref="A3"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C193" sqref="C193"/>
+      <selection pane="bottomRight" activeCell="C251" sqref="C251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
@@ -14706,7 +14706,7 @@
         <v>2350</v>
       </c>
       <c r="C190" s="17" t="s">
-        <v>2367</v>
+        <v>2366</v>
       </c>
       <c r="D190" s="16"/>
       <c r="E190" s="16" t="s">
@@ -14729,7 +14729,7 @@
         <v>2351</v>
       </c>
       <c r="C191" s="17" t="s">
-        <v>2368</v>
+        <v>2367</v>
       </c>
       <c r="D191" s="16"/>
       <c r="E191" s="16" t="s">
@@ -16306,7 +16306,7 @@
         <v>2319</v>
       </c>
       <c r="C250" s="47" t="s">
-        <v>2366</v>
+        <v>2368</v>
       </c>
       <c r="D250" s="24"/>
       <c r="E250" s="24" t="s">
@@ -33193,12 +33193,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100216A073BBB3FB3429D87D77C40313058" ma:contentTypeVersion="7" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="8cfc1d06a525c7d4ea1098b3952a2226">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="385505e6-e5d7-4f1a-b335-045f4e6272b3" xmlns:ns3="86b5f7f7-2f15-447a-b5f6-1e4312ec3a6d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="67eef51872945492eed3b93ded28523b" ns2:_="" ns3:_="">
     <xsd:import namespace="385505e6-e5d7-4f1a-b335-045f4e6272b3"/>
@@ -33381,6 +33375,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{430E6B59-185B-464E-889D-EBB334F9461E}">
   <ds:schemaRefs>
@@ -33390,23 +33390,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4AEB88-1F93-43C1-A78E-1A3EC40A664E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="aafb19fa-82be-411d-a6df-c75e9235a4ea"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="3dfebdfe-2b22-40ba-8672-9fbc9b4066c4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD65B255-3494-4F5F-976E-876698EF30C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33423,4 +33406,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4AEB88-1F93-43C1-A78E-1A3EC40A664E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="aafb19fa-82be-411d-a6df-c75e9235a4ea"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="3dfebdfe-2b22-40ba-8672-9fbc9b4066c4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>